<commit_message>
Importar RRegistros por nombre de columna
</commit_message>
<xml_diff>
--- a/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_InvActivo/Plantilla_InventarioActivo.xlsx
+++ b/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_InvActivo/Plantilla_InventarioActivo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waly_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waly_\source\repositorios\Supermercados\sistema-autorizadores\Web\SPSA.Autorizadores\SPSA.Autorizadores.Web\Plantillas_Tablas\Plantilla_InvActivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BD4138-CBBC-49A9-9A43-EE9A0725FE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FDFFC1-4B7D-4BC8-B248-ED9EAF045B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56FFDCFF-BA48-4534-97ED-533072800A9F}"/>
   </bookViews>
@@ -39,12 +39,6 @@
     <t>Sociedad</t>
   </si>
   <si>
-    <t>Nombre Sociedad</t>
-  </si>
-  <si>
-    <t>Ceco tda</t>
-  </si>
-  <si>
     <t>Tienda</t>
   </si>
   <si>
@@ -66,18 +60,9 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Área</t>
-  </si>
-  <si>
     <t>OC</t>
   </si>
   <si>
-    <t>GuÍa</t>
-  </si>
-  <si>
-    <t>Antigüedad</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -87,9 +72,6 @@
     <t>Garantia</t>
   </si>
   <si>
-    <t xml:space="preserve">Fecha actualización </t>
-  </si>
-  <si>
     <t>A125</t>
   </si>
   <si>
@@ -237,9 +219,6 @@
     <t>007-0061191</t>
   </si>
   <si>
-    <t>Fecha salida</t>
-  </si>
-  <si>
     <t>CodEmpresa</t>
   </si>
   <si>
@@ -301,6 +280,27 @@
   </si>
   <si>
     <t>290</t>
+  </si>
+  <si>
+    <t>NombreSociedad</t>
+  </si>
+  <si>
+    <t>Ceco</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Guia</t>
+  </si>
+  <si>
+    <t>FechaSalida</t>
+  </si>
+  <si>
+    <t>Antiguedad</t>
+  </si>
+  <si>
+    <t>FechaActualiza</t>
   </si>
 </sst>
 </file>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E553E5B-D34D-4BC9-8BB4-D16FA9F29797}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +785,7 @@
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
     <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -792,132 +793,132 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4">
         <v>25103011</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O2" s="5">
         <v>1</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
@@ -926,10 +927,10 @@
         <v>9</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
@@ -939,53 +940,53 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4">
         <v>25103011</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="K3" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="O3" s="5">
         <v>1</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
@@ -994,7 +995,7 @@
         <v>124</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
@@ -1005,43 +1006,43 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4">
         <v>24107029</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>84</v>
-      </c>
       <c r="K4" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N4" s="5">
         <v>31783494</v>
@@ -1050,16 +1051,16 @@
         <v>1</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="R4" s="5">
         <v>4200047886</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T4" s="6">
         <v>44379</v>
@@ -1068,13 +1069,13 @@
         <v>3</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="Y4" s="5"/>
       <c r="Z4" s="6">
@@ -1083,53 +1084,53 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4">
         <v>24107029</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="O5" s="5">
         <v>1</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
@@ -1140,7 +1141,7 @@
         <v>5</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -1151,57 +1152,57 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4">
         <v>24107029</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="O6" s="5">
         <v>1</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="T6" s="6">
         <v>44624</v>
@@ -1210,13 +1211,13 @@
         <v>2</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="Y6" s="5"/>
       <c r="Z6" s="6">
@@ -1225,59 +1226,59 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4">
         <v>24107029</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="O7" s="5">
         <v>1</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="T7" s="6">
         <v>44744</v>
@@ -1286,13 +1287,13 @@
         <v>2</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Y7" s="5"/>
       <c r="Z7" s="6">
@@ -1301,57 +1302,57 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
         <v>24107029</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="O8" s="5">
         <v>1</v>
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="T8" s="6">
         <v>44846</v>
@@ -1360,11 +1361,11 @@
         <v>2</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="W8" s="5"/>
       <c r="X8" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Y8" s="5"/>
       <c r="Z8" s="6">
@@ -1373,46 +1374,46 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4">
         <v>25104011</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O9" s="5">
         <v>1</v>
@@ -1421,7 +1422,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="T9" s="6">
         <v>44244</v>
@@ -1430,10 +1431,10 @@
         <v>3</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>

</xml_diff>